<commit_message>
Added exception catch for when output excel file is open
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -456,8 +456,26 @@
         <v>0</v>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Critical Path:</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>B -&gt; C</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>